<commit_message>
Created Outcome Columnb for games and added .csv files
</commit_message>
<xml_diff>
--- a/DataCleaning/Instat_DataCleaning/GamesCleaned.xlsx
+++ b/DataCleaning/Instat_DataCleaning/GamesCleaned.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:DI193"/>
+  <dimension ref="A1:DJ193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1003,6 +1003,11 @@
           <t>OpponentScore</t>
         </is>
       </c>
+      <c r="DJ1" s="1" t="inlineStr">
+        <is>
+          <t>Outcome</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -1348,6 +1353,11 @@
       <c r="DI2" t="n">
         <v>2</v>
       </c>
+      <c r="DJ2" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -1693,6 +1703,11 @@
       <c r="DI3" t="n">
         <v>4</v>
       </c>
+      <c r="DJ3" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -2038,6 +2053,11 @@
       <c r="DI4" t="n">
         <v>7</v>
       </c>
+      <c r="DJ4" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -2383,6 +2403,11 @@
       <c r="DI5" t="n">
         <v>1</v>
       </c>
+      <c r="DJ5" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -2728,6 +2753,11 @@
       <c r="DI6" t="n">
         <v>4</v>
       </c>
+      <c r="DJ6" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -3073,6 +3103,11 @@
       <c r="DI7" t="n">
         <v>1</v>
       </c>
+      <c r="DJ7" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -3418,6 +3453,11 @@
       <c r="DI8" t="n">
         <v>4</v>
       </c>
+      <c r="DJ8" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -3763,6 +3803,11 @@
       <c r="DI9" t="n">
         <v>0</v>
       </c>
+      <c r="DJ9" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -4108,6 +4153,11 @@
       <c r="DI10" t="n">
         <v>7</v>
       </c>
+      <c r="DJ10" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -4453,6 +4503,11 @@
       <c r="DI11" t="n">
         <v>4</v>
       </c>
+      <c r="DJ11" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -4798,6 +4853,11 @@
       <c r="DI12" t="n">
         <v>3</v>
       </c>
+      <c r="DJ12" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -5143,6 +5203,11 @@
       <c r="DI13" t="n">
         <v>2</v>
       </c>
+      <c r="DJ13" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -5488,6 +5553,11 @@
       <c r="DI14" t="n">
         <v>6</v>
       </c>
+      <c r="DJ14" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -5833,6 +5903,11 @@
       <c r="DI15" t="n">
         <v>2</v>
       </c>
+      <c r="DJ15" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -6178,6 +6253,11 @@
       <c r="DI16" t="n">
         <v>4</v>
       </c>
+      <c r="DJ16" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -6523,6 +6603,11 @@
       <c r="DI17" t="n">
         <v>3</v>
       </c>
+      <c r="DJ17" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -6868,6 +6953,11 @@
       <c r="DI18" t="n">
         <v>0</v>
       </c>
+      <c r="DJ18" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -7213,6 +7303,11 @@
       <c r="DI19" t="n">
         <v>1</v>
       </c>
+      <c r="DJ19" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -7558,6 +7653,11 @@
       <c r="DI20" t="n">
         <v>4</v>
       </c>
+      <c r="DJ20" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -7903,6 +8003,11 @@
       <c r="DI21" t="n">
         <v>1</v>
       </c>
+      <c r="DJ21" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -8248,6 +8353,11 @@
       <c r="DI22" t="n">
         <v>3</v>
       </c>
+      <c r="DJ22" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -8593,6 +8703,11 @@
       <c r="DI23" t="n">
         <v>0</v>
       </c>
+      <c r="DJ23" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -8938,6 +9053,11 @@
       <c r="DI24" t="n">
         <v>7</v>
       </c>
+      <c r="DJ24" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -9283,6 +9403,11 @@
       <c r="DI25" t="n">
         <v>3</v>
       </c>
+      <c r="DJ25" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -9628,6 +9753,11 @@
       <c r="DI26" t="n">
         <v>3</v>
       </c>
+      <c r="DJ26" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -9973,6 +10103,11 @@
       <c r="DI27" t="n">
         <v>0</v>
       </c>
+      <c r="DJ27" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -10318,6 +10453,11 @@
       <c r="DI28" t="n">
         <v>4</v>
       </c>
+      <c r="DJ28" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -10663,6 +10803,11 @@
       <c r="DI29" t="n">
         <v>1</v>
       </c>
+      <c r="DJ29" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -11008,6 +11153,11 @@
       <c r="DI30" t="n">
         <v>0</v>
       </c>
+      <c r="DJ30" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -11353,6 +11503,11 @@
       <c r="DI31" t="n">
         <v>3</v>
       </c>
+      <c r="DJ31" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -11698,6 +11853,11 @@
       <c r="DI32" t="n">
         <v>2</v>
       </c>
+      <c r="DJ32" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -12043,6 +12203,11 @@
       <c r="DI33" t="n">
         <v>1</v>
       </c>
+      <c r="DJ33" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -12388,6 +12553,11 @@
       <c r="DI34" t="n">
         <v>2</v>
       </c>
+      <c r="DJ34" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -12733,6 +12903,11 @@
       <c r="DI35" t="n">
         <v>1</v>
       </c>
+      <c r="DJ35" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -13078,6 +13253,11 @@
       <c r="DI36" t="n">
         <v>7</v>
       </c>
+      <c r="DJ36" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -13423,6 +13603,11 @@
       <c r="DI37" t="n">
         <v>1</v>
       </c>
+      <c r="DJ37" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -13768,6 +13953,11 @@
       <c r="DI38" t="n">
         <v>5</v>
       </c>
+      <c r="DJ38" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -14113,6 +14303,11 @@
       <c r="DI39" t="n">
         <v>0</v>
       </c>
+      <c r="DJ39" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -14458,6 +14653,11 @@
       <c r="DI40" t="n">
         <v>4</v>
       </c>
+      <c r="DJ40" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -14803,6 +15003,11 @@
       <c r="DI41" t="n">
         <v>1</v>
       </c>
+      <c r="DJ41" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -15148,6 +15353,11 @@
       <c r="DI42" t="n">
         <v>4</v>
       </c>
+      <c r="DJ42" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -15493,6 +15703,11 @@
       <c r="DI43" t="n">
         <v>0</v>
       </c>
+      <c r="DJ43" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -15838,6 +16053,11 @@
       <c r="DI44" t="n">
         <v>3</v>
       </c>
+      <c r="DJ44" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -16183,6 +16403,11 @@
       <c r="DI45" t="n">
         <v>1</v>
       </c>
+      <c r="DJ45" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -16528,6 +16753,11 @@
       <c r="DI46" t="n">
         <v>3</v>
       </c>
+      <c r="DJ46" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -16873,6 +17103,11 @@
       <c r="DI47" t="n">
         <v>4</v>
       </c>
+      <c r="DJ47" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -17218,6 +17453,11 @@
       <c r="DI48" t="n">
         <v>2</v>
       </c>
+      <c r="DJ48" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -17563,6 +17803,11 @@
       <c r="DI49" t="n">
         <v>3</v>
       </c>
+      <c r="DJ49" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
@@ -17908,6 +18153,11 @@
       <c r="DI50" t="n">
         <v>2</v>
       </c>
+      <c r="DJ50" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
@@ -18253,6 +18503,11 @@
       <c r="DI51" t="n">
         <v>4</v>
       </c>
+      <c r="DJ51" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
@@ -18598,6 +18853,11 @@
       <c r="DI52" t="n">
         <v>7</v>
       </c>
+      <c r="DJ52" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
@@ -18943,6 +19203,11 @@
       <c r="DI53" t="n">
         <v>1</v>
       </c>
+      <c r="DJ53" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
@@ -19288,6 +19553,11 @@
       <c r="DI54" t="n">
         <v>4</v>
       </c>
+      <c r="DJ54" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
@@ -19633,6 +19903,11 @@
       <c r="DI55" t="n">
         <v>1</v>
       </c>
+      <c r="DJ55" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
@@ -19978,6 +20253,11 @@
       <c r="DI56" t="n">
         <v>4</v>
       </c>
+      <c r="DJ56" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
@@ -20323,6 +20603,11 @@
       <c r="DI57" t="n">
         <v>0</v>
       </c>
+      <c r="DJ57" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
@@ -20668,6 +20953,11 @@
       <c r="DI58" t="n">
         <v>7</v>
       </c>
+      <c r="DJ58" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
@@ -21013,6 +21303,11 @@
       <c r="DI59" t="n">
         <v>4</v>
       </c>
+      <c r="DJ59" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
@@ -21358,6 +21653,11 @@
       <c r="DI60" t="n">
         <v>3</v>
       </c>
+      <c r="DJ60" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
@@ -21703,6 +22003,11 @@
       <c r="DI61" t="n">
         <v>2</v>
       </c>
+      <c r="DJ61" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
@@ -22048,6 +22353,11 @@
       <c r="DI62" t="n">
         <v>6</v>
       </c>
+      <c r="DJ62" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
@@ -22393,6 +22703,11 @@
       <c r="DI63" t="n">
         <v>2</v>
       </c>
+      <c r="DJ63" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
@@ -22738,6 +23053,11 @@
       <c r="DI64" t="n">
         <v>4</v>
       </c>
+      <c r="DJ64" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
@@ -23083,6 +23403,11 @@
       <c r="DI65" t="n">
         <v>3</v>
       </c>
+      <c r="DJ65" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
@@ -23428,6 +23753,11 @@
       <c r="DI66" t="n">
         <v>0</v>
       </c>
+      <c r="DJ66" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
@@ -23773,6 +24103,11 @@
       <c r="DI67" t="n">
         <v>1</v>
       </c>
+      <c r="DJ67" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
@@ -24118,6 +24453,11 @@
       <c r="DI68" t="n">
         <v>4</v>
       </c>
+      <c r="DJ68" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
@@ -24463,6 +24803,11 @@
       <c r="DI69" t="n">
         <v>1</v>
       </c>
+      <c r="DJ69" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
@@ -24808,6 +25153,11 @@
       <c r="DI70" t="n">
         <v>3</v>
       </c>
+      <c r="DJ70" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
@@ -25153,6 +25503,11 @@
       <c r="DI71" t="n">
         <v>0</v>
       </c>
+      <c r="DJ71" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
@@ -25498,6 +25853,11 @@
       <c r="DI72" t="n">
         <v>7</v>
       </c>
+      <c r="DJ72" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
@@ -25843,6 +26203,11 @@
       <c r="DI73" t="n">
         <v>3</v>
       </c>
+      <c r="DJ73" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
@@ -26188,6 +26553,11 @@
       <c r="DI74" t="n">
         <v>3</v>
       </c>
+      <c r="DJ74" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
@@ -26533,6 +26903,11 @@
       <c r="DI75" t="n">
         <v>0</v>
       </c>
+      <c r="DJ75" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
@@ -26878,6 +27253,11 @@
       <c r="DI76" t="n">
         <v>4</v>
       </c>
+      <c r="DJ76" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
@@ -27223,6 +27603,11 @@
       <c r="DI77" t="n">
         <v>1</v>
       </c>
+      <c r="DJ77" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -27568,6 +27953,11 @@
       <c r="DI78" t="n">
         <v>0</v>
       </c>
+      <c r="DJ78" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
@@ -27913,6 +28303,11 @@
       <c r="DI79" t="n">
         <v>3</v>
       </c>
+      <c r="DJ79" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
@@ -28258,6 +28653,11 @@
       <c r="DI80" t="n">
         <v>2</v>
       </c>
+      <c r="DJ80" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
@@ -28603,6 +29003,11 @@
       <c r="DI81" t="n">
         <v>1</v>
       </c>
+      <c r="DJ81" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
@@ -28948,6 +29353,11 @@
       <c r="DI82" t="n">
         <v>2</v>
       </c>
+      <c r="DJ82" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
@@ -29293,6 +29703,11 @@
       <c r="DI83" t="n">
         <v>1</v>
       </c>
+      <c r="DJ83" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
@@ -29638,6 +30053,11 @@
       <c r="DI84" t="n">
         <v>7</v>
       </c>
+      <c r="DJ84" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
@@ -29983,6 +30403,11 @@
       <c r="DI85" t="n">
         <v>1</v>
       </c>
+      <c r="DJ85" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
@@ -30328,6 +30753,11 @@
       <c r="DI86" t="n">
         <v>5</v>
       </c>
+      <c r="DJ86" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
@@ -30673,6 +31103,11 @@
       <c r="DI87" t="n">
         <v>0</v>
       </c>
+      <c r="DJ87" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
@@ -31018,6 +31453,11 @@
       <c r="DI88" t="n">
         <v>4</v>
       </c>
+      <c r="DJ88" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
@@ -31363,6 +31803,11 @@
       <c r="DI89" t="n">
         <v>1</v>
       </c>
+      <c r="DJ89" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
@@ -31708,6 +32153,11 @@
       <c r="DI90" t="n">
         <v>4</v>
       </c>
+      <c r="DJ90" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
@@ -32053,6 +32503,11 @@
       <c r="DI91" t="n">
         <v>0</v>
       </c>
+      <c r="DJ91" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
@@ -32398,6 +32853,11 @@
       <c r="DI92" t="n">
         <v>3</v>
       </c>
+      <c r="DJ92" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
@@ -32743,6 +33203,11 @@
       <c r="DI93" t="n">
         <v>1</v>
       </c>
+      <c r="DJ93" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
@@ -33088,6 +33553,11 @@
       <c r="DI94" t="n">
         <v>3</v>
       </c>
+      <c r="DJ94" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
@@ -33433,6 +33903,11 @@
       <c r="DI95" t="n">
         <v>4</v>
       </c>
+      <c r="DJ95" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
@@ -33778,6 +34253,11 @@
       <c r="DI96" t="n">
         <v>2</v>
       </c>
+      <c r="DJ96" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
@@ -34123,6 +34603,11 @@
       <c r="DI97" t="n">
         <v>3</v>
       </c>
+      <c r="DJ97" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
@@ -34468,6 +34953,11 @@
       <c r="DI98" t="n">
         <v>2</v>
       </c>
+      <c r="DJ98" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
@@ -34813,6 +35303,11 @@
       <c r="DI99" t="n">
         <v>4</v>
       </c>
+      <c r="DJ99" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
@@ -35158,6 +35653,11 @@
       <c r="DI100" t="n">
         <v>7</v>
       </c>
+      <c r="DJ100" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
@@ -35503,6 +36003,11 @@
       <c r="DI101" t="n">
         <v>1</v>
       </c>
+      <c r="DJ101" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
@@ -35848,6 +36353,11 @@
       <c r="DI102" t="n">
         <v>4</v>
       </c>
+      <c r="DJ102" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
@@ -36193,6 +36703,11 @@
       <c r="DI103" t="n">
         <v>1</v>
       </c>
+      <c r="DJ103" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
@@ -36538,6 +37053,11 @@
       <c r="DI104" t="n">
         <v>4</v>
       </c>
+      <c r="DJ104" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
@@ -36883,6 +37403,11 @@
       <c r="DI105" t="n">
         <v>0</v>
       </c>
+      <c r="DJ105" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
@@ -37228,6 +37753,11 @@
       <c r="DI106" t="n">
         <v>7</v>
       </c>
+      <c r="DJ106" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
@@ -37573,6 +38103,11 @@
       <c r="DI107" t="n">
         <v>4</v>
       </c>
+      <c r="DJ107" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
@@ -37918,6 +38453,11 @@
       <c r="DI108" t="n">
         <v>3</v>
       </c>
+      <c r="DJ108" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
@@ -38263,6 +38803,11 @@
       <c r="DI109" t="n">
         <v>2</v>
       </c>
+      <c r="DJ109" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
@@ -38608,6 +39153,11 @@
       <c r="DI110" t="n">
         <v>6</v>
       </c>
+      <c r="DJ110" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
@@ -38953,6 +39503,11 @@
       <c r="DI111" t="n">
         <v>2</v>
       </c>
+      <c r="DJ111" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
@@ -39298,6 +39853,11 @@
       <c r="DI112" t="n">
         <v>4</v>
       </c>
+      <c r="DJ112" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
@@ -39643,6 +40203,11 @@
       <c r="DI113" t="n">
         <v>3</v>
       </c>
+      <c r="DJ113" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
@@ -39988,6 +40553,11 @@
       <c r="DI114" t="n">
         <v>0</v>
       </c>
+      <c r="DJ114" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
@@ -40333,6 +40903,11 @@
       <c r="DI115" t="n">
         <v>1</v>
       </c>
+      <c r="DJ115" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
@@ -40678,6 +41253,11 @@
       <c r="DI116" t="n">
         <v>4</v>
       </c>
+      <c r="DJ116" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
@@ -41023,6 +41603,11 @@
       <c r="DI117" t="n">
         <v>1</v>
       </c>
+      <c r="DJ117" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
@@ -41368,6 +41953,11 @@
       <c r="DI118" t="n">
         <v>3</v>
       </c>
+      <c r="DJ118" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
@@ -41713,6 +42303,11 @@
       <c r="DI119" t="n">
         <v>0</v>
       </c>
+      <c r="DJ119" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
@@ -42058,6 +42653,11 @@
       <c r="DI120" t="n">
         <v>7</v>
       </c>
+      <c r="DJ120" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
@@ -42403,6 +43003,11 @@
       <c r="DI121" t="n">
         <v>3</v>
       </c>
+      <c r="DJ121" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
@@ -42748,6 +43353,11 @@
       <c r="DI122" t="n">
         <v>3</v>
       </c>
+      <c r="DJ122" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
@@ -43093,6 +43703,11 @@
       <c r="DI123" t="n">
         <v>0</v>
       </c>
+      <c r="DJ123" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
@@ -43438,6 +44053,11 @@
       <c r="DI124" t="n">
         <v>4</v>
       </c>
+      <c r="DJ124" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
@@ -43783,6 +44403,11 @@
       <c r="DI125" t="n">
         <v>1</v>
       </c>
+      <c r="DJ125" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
@@ -44128,6 +44753,11 @@
       <c r="DI126" t="n">
         <v>0</v>
       </c>
+      <c r="DJ126" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
@@ -44473,6 +45103,11 @@
       <c r="DI127" t="n">
         <v>3</v>
       </c>
+      <c r="DJ127" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
@@ -44818,6 +45453,11 @@
       <c r="DI128" t="n">
         <v>2</v>
       </c>
+      <c r="DJ128" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
@@ -45163,6 +45803,11 @@
       <c r="DI129" t="n">
         <v>1</v>
       </c>
+      <c r="DJ129" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
@@ -45508,6 +46153,11 @@
       <c r="DI130" t="n">
         <v>2</v>
       </c>
+      <c r="DJ130" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
@@ -45853,6 +46503,11 @@
       <c r="DI131" t="n">
         <v>1</v>
       </c>
+      <c r="DJ131" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
@@ -46198,6 +46853,11 @@
       <c r="DI132" t="n">
         <v>7</v>
       </c>
+      <c r="DJ132" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
@@ -46543,6 +47203,11 @@
       <c r="DI133" t="n">
         <v>1</v>
       </c>
+      <c r="DJ133" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
@@ -46888,6 +47553,11 @@
       <c r="DI134" t="n">
         <v>5</v>
       </c>
+      <c r="DJ134" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
@@ -47233,6 +47903,11 @@
       <c r="DI135" t="n">
         <v>0</v>
       </c>
+      <c r="DJ135" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
@@ -47578,6 +48253,11 @@
       <c r="DI136" t="n">
         <v>4</v>
       </c>
+      <c r="DJ136" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
@@ -47923,6 +48603,11 @@
       <c r="DI137" t="n">
         <v>1</v>
       </c>
+      <c r="DJ137" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
@@ -48268,6 +48953,11 @@
       <c r="DI138" t="n">
         <v>4</v>
       </c>
+      <c r="DJ138" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
@@ -48613,6 +49303,11 @@
       <c r="DI139" t="n">
         <v>0</v>
       </c>
+      <c r="DJ139" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
@@ -48958,6 +49653,11 @@
       <c r="DI140" t="n">
         <v>3</v>
       </c>
+      <c r="DJ140" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
@@ -49303,6 +50003,11 @@
       <c r="DI141" t="n">
         <v>1</v>
       </c>
+      <c r="DJ141" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
@@ -49648,6 +50353,11 @@
       <c r="DI142" t="n">
         <v>3</v>
       </c>
+      <c r="DJ142" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
@@ -49993,6 +50703,11 @@
       <c r="DI143" t="n">
         <v>4</v>
       </c>
+      <c r="DJ143" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
@@ -50338,6 +51053,11 @@
       <c r="DI144" t="n">
         <v>2</v>
       </c>
+      <c r="DJ144" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
@@ -50683,6 +51403,11 @@
       <c r="DI145" t="n">
         <v>3</v>
       </c>
+      <c r="DJ145" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
@@ -51028,6 +51753,11 @@
       <c r="DI146" t="n">
         <v>2</v>
       </c>
+      <c r="DJ146" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
@@ -51373,6 +52103,11 @@
       <c r="DI147" t="n">
         <v>4</v>
       </c>
+      <c r="DJ147" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
@@ -51718,6 +52453,11 @@
       <c r="DI148" t="n">
         <v>7</v>
       </c>
+      <c r="DJ148" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
@@ -52063,6 +52803,11 @@
       <c r="DI149" t="n">
         <v>1</v>
       </c>
+      <c r="DJ149" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
@@ -52408,6 +53153,11 @@
       <c r="DI150" t="n">
         <v>4</v>
       </c>
+      <c r="DJ150" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
@@ -52753,6 +53503,11 @@
       <c r="DI151" t="n">
         <v>1</v>
       </c>
+      <c r="DJ151" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
@@ -53098,6 +53853,11 @@
       <c r="DI152" t="n">
         <v>4</v>
       </c>
+      <c r="DJ152" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
@@ -53443,6 +54203,11 @@
       <c r="DI153" t="n">
         <v>0</v>
       </c>
+      <c r="DJ153" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
@@ -53788,6 +54553,11 @@
       <c r="DI154" t="n">
         <v>7</v>
       </c>
+      <c r="DJ154" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
@@ -54133,6 +54903,11 @@
       <c r="DI155" t="n">
         <v>4</v>
       </c>
+      <c r="DJ155" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
@@ -54478,6 +55253,11 @@
       <c r="DI156" t="n">
         <v>3</v>
       </c>
+      <c r="DJ156" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
@@ -54823,6 +55603,11 @@
       <c r="DI157" t="n">
         <v>2</v>
       </c>
+      <c r="DJ157" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
@@ -55168,6 +55953,11 @@
       <c r="DI158" t="n">
         <v>6</v>
       </c>
+      <c r="DJ158" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
@@ -55513,6 +56303,11 @@
       <c r="DI159" t="n">
         <v>2</v>
       </c>
+      <c r="DJ159" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
@@ -55858,6 +56653,11 @@
       <c r="DI160" t="n">
         <v>4</v>
       </c>
+      <c r="DJ160" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
@@ -56203,6 +57003,11 @@
       <c r="DI161" t="n">
         <v>3</v>
       </c>
+      <c r="DJ161" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
@@ -56548,6 +57353,11 @@
       <c r="DI162" t="n">
         <v>0</v>
       </c>
+      <c r="DJ162" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
@@ -56893,6 +57703,11 @@
       <c r="DI163" t="n">
         <v>1</v>
       </c>
+      <c r="DJ163" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
@@ -57238,6 +58053,11 @@
       <c r="DI164" t="n">
         <v>4</v>
       </c>
+      <c r="DJ164" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
@@ -57583,6 +58403,11 @@
       <c r="DI165" t="n">
         <v>1</v>
       </c>
+      <c r="DJ165" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
@@ -57928,6 +58753,11 @@
       <c r="DI166" t="n">
         <v>3</v>
       </c>
+      <c r="DJ166" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
@@ -58273,6 +59103,11 @@
       <c r="DI167" t="n">
         <v>0</v>
       </c>
+      <c r="DJ167" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
@@ -58618,6 +59453,11 @@
       <c r="DI168" t="n">
         <v>7</v>
       </c>
+      <c r="DJ168" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
@@ -58963,6 +59803,11 @@
       <c r="DI169" t="n">
         <v>3</v>
       </c>
+      <c r="DJ169" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
@@ -59308,6 +60153,11 @@
       <c r="DI170" t="n">
         <v>3</v>
       </c>
+      <c r="DJ170" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="2" t="n">
@@ -59653,6 +60503,11 @@
       <c r="DI171" t="n">
         <v>0</v>
       </c>
+      <c r="DJ171" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="2" t="n">
@@ -59998,6 +60853,11 @@
       <c r="DI172" t="n">
         <v>4</v>
       </c>
+      <c r="DJ172" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="2" t="n">
@@ -60343,6 +61203,11 @@
       <c r="DI173" t="n">
         <v>1</v>
       </c>
+      <c r="DJ173" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="2" t="n">
@@ -60688,6 +61553,11 @@
       <c r="DI174" t="n">
         <v>0</v>
       </c>
+      <c r="DJ174" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="2" t="n">
@@ -61033,6 +61903,11 @@
       <c r="DI175" t="n">
         <v>3</v>
       </c>
+      <c r="DJ175" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="2" t="n">
@@ -61378,6 +62253,11 @@
       <c r="DI176" t="n">
         <v>2</v>
       </c>
+      <c r="DJ176" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="2" t="n">
@@ -61723,6 +62603,11 @@
       <c r="DI177" t="n">
         <v>1</v>
       </c>
+      <c r="DJ177" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="2" t="n">
@@ -62068,6 +62953,11 @@
       <c r="DI178" t="n">
         <v>2</v>
       </c>
+      <c r="DJ178" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="2" t="n">
@@ -62413,6 +63303,11 @@
       <c r="DI179" t="n">
         <v>1</v>
       </c>
+      <c r="DJ179" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="2" t="n">
@@ -62758,6 +63653,11 @@
       <c r="DI180" t="n">
         <v>7</v>
       </c>
+      <c r="DJ180" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="2" t="n">
@@ -63103,6 +64003,11 @@
       <c r="DI181" t="n">
         <v>1</v>
       </c>
+      <c r="DJ181" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
@@ -63448,6 +64353,11 @@
       <c r="DI182" t="n">
         <v>5</v>
       </c>
+      <c r="DJ182" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="n">
@@ -63793,6 +64703,11 @@
       <c r="DI183" t="n">
         <v>0</v>
       </c>
+      <c r="DJ183" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="2" t="n">
@@ -64138,6 +65053,11 @@
       <c r="DI184" t="n">
         <v>4</v>
       </c>
+      <c r="DJ184" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="2" t="n">
@@ -64483,6 +65403,11 @@
       <c r="DI185" t="n">
         <v>1</v>
       </c>
+      <c r="DJ185" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="2" t="n">
@@ -64828,6 +65753,11 @@
       <c r="DI186" t="n">
         <v>4</v>
       </c>
+      <c r="DJ186" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="2" t="n">
@@ -65173,6 +66103,11 @@
       <c r="DI187" t="n">
         <v>0</v>
       </c>
+      <c r="DJ187" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="2" t="n">
@@ -65518,6 +66453,11 @@
       <c r="DI188" t="n">
         <v>3</v>
       </c>
+      <c r="DJ188" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="2" t="n">
@@ -65863,6 +66803,11 @@
       <c r="DI189" t="n">
         <v>1</v>
       </c>
+      <c r="DJ189" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="n">
@@ -66208,6 +67153,11 @@
       <c r="DI190" t="n">
         <v>3</v>
       </c>
+      <c r="DJ190" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="2" t="n">
@@ -66553,6 +67503,11 @@
       <c r="DI191" t="n">
         <v>4</v>
       </c>
+      <c r="DJ191" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="2" t="n">
@@ -66898,6 +67853,11 @@
       <c r="DI192" t="n">
         <v>2</v>
       </c>
+      <c r="DJ192" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="2" t="n">
@@ -67242,6 +68202,11 @@
       </c>
       <c r="DI193" t="n">
         <v>3</v>
+      </c>
+      <c r="DJ193" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>